<commit_message>
Refactor ToolListEditor layout for enhanced part image display and PDF export consistency
- Adjusted dimensions and alignment of part image boxes to improve visual representation.
- Enhanced layout consistency for part images and tool specifications during PDF exports, ensuring a polished document appearance.
</commit_message>
<xml_diff>
--- a/CNCToolingDatabase/Data/MASTER - MACHINE MODEL.xlsx
+++ b/CNCToolingDatabase/Data/MASTER - MACHINE MODEL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Tool-Master-Control\Tool-Master-Control\CNCToolingDatabase\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7833CD-BD68-403B-B996-286761F42CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA1FD54-7656-4096-B1CF-7F7EF5584558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{8271D9D6-2065-419F-AC52-7850B71D4074}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8271D9D6-2065-419F-AC52-7850B71D4074}"/>
   </bookViews>
   <sheets>
     <sheet name="Machine_Model" sheetId="1" r:id="rId1"/>
@@ -144,9 +144,6 @@
     <t>HCN6000 II</t>
   </si>
   <si>
-    <t>HTC 4000-II</t>
-  </si>
-  <si>
     <t>HiREX-4000</t>
   </si>
   <si>
@@ -310,6 +307,9 @@
   </si>
   <si>
     <t>MYNX9500</t>
+  </si>
+  <si>
+    <t>HTC4000-II</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1F9D2975-A917-404F-9FF3-664FDE891014}" name="Table1" displayName="Table1" ref="A1:F66" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:F66" xr:uid="{1F9D2975-A917-404F-9FF3-664FDE891014}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F66">
-    <sortCondition ref="A1:A66"/>
+    <sortCondition ref="B1:B66"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{4A87BED8-B1B5-45DE-BB4C-8C3E6116591E}" name="No." dataDxfId="5"/>
@@ -800,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8EBE31-42AA-4644-A64F-E2B9900B290E}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,13 +1202,13 @@
         <v>36</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>2</v>
@@ -1219,16 +1219,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>2</v>
@@ -1239,13 +1239,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>32</v>
@@ -1259,13 +1259,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>32</v>
@@ -1279,13 +1279,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>32</v>
@@ -1299,13 +1299,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>32</v>
@@ -1319,7 +1319,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>22</v>
@@ -1339,16 +1339,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>2</v>
@@ -1359,7 +1359,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>12</v>
@@ -1368,7 +1368,7 @@
         <v>9</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>2</v>
@@ -1379,7 +1379,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>12</v>
@@ -1388,7 +1388,7 @@
         <v>9</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>2</v>
@@ -1399,7 +1399,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>12</v>
@@ -1408,7 +1408,7 @@
         <v>9</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>2</v>
@@ -1419,7 +1419,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>12</v>
@@ -1428,7 +1428,7 @@
         <v>9</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>2</v>
@@ -1439,7 +1439,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>31</v>
@@ -1459,13 +1459,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>32</v>
@@ -1479,13 +1479,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>32</v>
@@ -1499,13 +1499,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
@@ -1519,13 +1519,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>32</v>
@@ -1539,13 +1539,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>32</v>
@@ -1559,13 +1559,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>32</v>
@@ -1579,13 +1579,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>32</v>
@@ -1599,10 +1599,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>9</v>
@@ -1619,10 +1619,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>9</v>
@@ -1639,10 +1639,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>9</v>
@@ -1659,10 +1659,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>9</v>
@@ -1679,10 +1679,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>9</v>
@@ -1699,13 +1699,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="D45" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>13</v>
@@ -1719,16 +1719,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="D46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>2</v>
@@ -1742,13 +1742,13 @@
         <v>70</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>2</v>
@@ -1762,13 +1762,13 @@
         <v>71</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>2</v>
@@ -1779,16 +1779,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>2</v>
@@ -1799,7 +1799,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>31</v>
@@ -1819,7 +1819,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>31</v>
@@ -1839,7 +1839,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>31</v>
@@ -1859,7 +1859,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>31</v>
@@ -1879,7 +1879,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>31</v>
@@ -1899,7 +1899,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>31</v>
@@ -1919,7 +1919,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>31</v>
@@ -1939,7 +1939,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>31</v>
@@ -1959,7 +1959,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>31</v>
@@ -1979,7 +1979,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>31</v>
@@ -1999,7 +1999,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>31</v>
@@ -2019,16 +2019,16 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>2</v>
@@ -2039,7 +2039,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>31</v>
@@ -2059,7 +2059,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>31</v>
@@ -2079,7 +2079,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>31</v>
@@ -2099,16 +2099,16 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>89</v>
+        <v>31</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>2</v>
@@ -2119,7 +2119,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Enhance ToolListEditor layout and image handling for improved PDF exports
- Refined layout of part image boxes in the ToolListEditor for better visual representation and alignment.
- Improved image loading logic to ensure consistent display of part images during PDF generation, enhancing overall document quality.
- Adjusted dimensions and styles for part images to maintain a polished appearance in exports.
</commit_message>
<xml_diff>
--- a/CNCToolingDatabase/Data/MASTER - MACHINE MODEL.xlsx
+++ b/CNCToolingDatabase/Data/MASTER - MACHINE MODEL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Tool-Master-Control\Tool-Master-Control\CNCToolingDatabase\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA1FD54-7656-4096-B1CF-7F7EF5584558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5199E5E-8DD2-4ECB-B7BF-C87997D3333E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8271D9D6-2065-419F-AC52-7850B71D4074}"/>
   </bookViews>
@@ -359,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -371,6 +371,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -800,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8EBE31-42AA-4644-A64F-E2B9900B290E}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A66"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,23 +1200,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+    <row r="20" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="D20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="6" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>